<commit_message>
create method: delete cookie
</commit_message>
<xml_diff>
--- a/Заказ.xlsx
+++ b/Заказ.xlsx
@@ -34,16 +34,16 @@
     <t>итоговая цена</t>
   </si>
   <si>
-    <t>Толстовка красканая</t>
-  </si>
-  <si>
-    <t>красный</t>
+    <t>Худи Зеленая</t>
+  </si>
+  <si>
+    <t>зеленый</t>
+  </si>
+  <si>
+    <t>XL</t>
   </si>
   <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>S</t>
   </si>
   <si>
     <t>+7 (937) 465 56 89</t>
@@ -469,7 +469,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -503,7 +503,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="2">
-        <v>10000</v>
+        <v>8000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update auth and guard
</commit_message>
<xml_diff>
--- a/Заказ.xlsx
+++ b/Заказ.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Название товара</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>XL</t>
-  </si>
-  <si>
-    <t>S</t>
   </si>
   <si>
     <t>+7 (937) 465 56 89</t>
@@ -433,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="40" style="1" customWidth="1"/>
@@ -481,29 +478,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="3" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2">
         <v>1000</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>